<commit_message>
Add test cases Set up data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/lucy_data_driven_test/testdata.xlsx
+++ b/src/test/resources/excel/lucy_data_driven_test/testdata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\Batch22ndJuly2018WebDriver\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\seleniumjava\src\test\resources\excel\lucy_data_driven_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{84F681A0-D961-4E9D-A8F0-5858CA40FD9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{0E5FAE3A-4BD0-424C-A182-C1E242C68389}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="17250" windowHeight="5655"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="2" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>firstname</t>
   </si>
@@ -37,37 +36,28 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>A234234</t>
-  </si>
-  <si>
     <t>customer</t>
   </si>
   <si>
     <t>currency</t>
   </si>
   <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
+    <t>dang</t>
+  </si>
+  <si>
+    <t>chau</t>
+  </si>
+  <si>
+    <t>dang chau</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,16 +402,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC866097-B634-4C4A-9D8A-AD659098FF52}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,22 +424,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -455,29 +442,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C183F-55DE-44A5-835D-B4C14A682D86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Config capture to work with maven sure-fire plugin folder
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/lucy_data_driven_test/testdata.xlsx
+++ b/src/test/resources/excel/lucy_data_driven_test/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="17250" windowHeight="5655"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="17250" windowHeight="5655"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>firstname</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Dollar</t>
+  </si>
+  <si>
+    <t>alertmessage</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +420,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +430,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -434,6 +443,9 @@
       </c>
       <c r="C2">
         <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>